<commit_message>
Harkat 4 ja 5 lisätty
</commit_message>
<xml_diff>
--- a/harkat/harkat_pohja.xlsx
+++ b/harkat/harkat_pohja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuni-my.sharepoint.com/personal/teemu_helenius_tuni_fi/Documents/Yrityksen talous/tiiviste/harkat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{89EAE0E3-53EA-4691-BDD9-A76C84E4BCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B87503F-E916-428D-B16F-D18BD514D1D0}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="8_{89EAE0E3-53EA-4691-BDD9-A76C84E4BCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0AC4C0B4-AE07-42A8-95F7-0792B8A19800}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
   <si>
     <t>Kassa</t>
   </si>
@@ -145,6 +145,126 @@
   </si>
   <si>
     <t>Taseen loppusumma =</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>Palkat</t>
+  </si>
+  <si>
+    <t>Pankkitili</t>
+  </si>
+  <si>
+    <t>Siirtosaamiset</t>
+  </si>
+  <si>
+    <t>Sosiaalimenot</t>
+  </si>
+  <si>
+    <t>Konttorimenot</t>
+  </si>
+  <si>
+    <t>Vuokrat</t>
+  </si>
+  <si>
+    <t>K14</t>
+  </si>
+  <si>
+    <t>K32</t>
+  </si>
+  <si>
+    <t>VOM inventointimenettelyllä (Harkassa arvot pyöristetty)</t>
+  </si>
+  <si>
+    <t>Vöiden arvo</t>
+  </si>
+  <si>
+    <t>Lompakoiden arvo</t>
+  </si>
+  <si>
+    <t>Raaka-aineen arvo</t>
+  </si>
+  <si>
+    <t>Yhteensä</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Tilikauden voitto</t>
+  </si>
+  <si>
+    <t>10% tasapoisto = ?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>b:n) kirjaukset</t>
+  </si>
+  <si>
+    <t>Vuokra jaksotettuna</t>
+  </si>
+  <si>
+    <t>Myynti- ja siirtosaamiset</t>
+  </si>
+  <si>
+    <t>Palkat + sosiaalimenot</t>
+  </si>
+  <si>
+    <t>Vuokrat + konttorimenot</t>
+  </si>
+  <si>
+    <t>Liikevaihto (=myynti)</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>Materiaalit ja palvelut</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Ostot tilikauden aikana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Varastojen muutos</t>
+  </si>
+  <si>
+    <t>Henkilöstökulut</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Palkat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ..</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Muut henkilösivukulut</t>
+  </si>
+  <si>
+    <t>Poistot ja arvonalentumiset</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Suunnitelman mukaiset poistot</t>
+  </si>
+  <si>
+    <t>Liiketoiminnan muut kulut</t>
+  </si>
+  <si>
+    <t>Liikevoitto</t>
+  </si>
+  <si>
+    <t>Tilinpäätös</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
   </si>
 </sst>
 </file>
@@ -160,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,8 +293,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -222,17 +348,134 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -248,6 +491,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>182841</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Kuva 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74E149B5-6767-41AD-A32E-03FB4A4DB137}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="23060026"/>
+          <a:ext cx="5838825" cy="6459815"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,14 +822,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AM42"/>
+  <dimension ref="A1:AM159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="L155" sqref="L155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
@@ -849,7 +1163,7 @@
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1002,7 +1316,7 @@
       <c r="AI32" s="3"/>
       <c r="AL32" s="3"/>
     </row>
-    <row r="33" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
       <c r="E33" s="3"/>
       <c r="H33" s="3"/>
@@ -1017,7 +1331,7 @@
       <c r="AI33" s="3"/>
       <c r="AL33" s="3"/>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="E34" s="3"/>
       <c r="H34" s="3"/>
@@ -1032,7 +1346,7 @@
       <c r="AI34" s="3"/>
       <c r="AL34" s="3"/>
     </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="E35" s="3"/>
       <c r="H35" s="3"/>
@@ -1047,7 +1361,7 @@
       <c r="AI35" s="3"/>
       <c r="AL35" s="3"/>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="E36" s="3"/>
       <c r="H36" s="3"/>
@@ -1062,7 +1376,7 @@
       <c r="AI36" s="3"/>
       <c r="AL36" s="3"/>
     </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="E37" s="3"/>
       <c r="H37" s="3"/>
@@ -1077,7 +1391,7 @@
       <c r="AI37" s="3"/>
       <c r="AL37" s="3"/>
     </row>
-    <row r="38" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="E38" s="3"/>
       <c r="H38" s="3"/>
@@ -1092,7 +1406,7 @@
       <c r="AI38" s="3"/>
       <c r="AL38" s="3"/>
     </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="E39" s="3"/>
       <c r="H39" s="3"/>
@@ -1107,7 +1421,7 @@
       <c r="AI39" s="3"/>
       <c r="AL39" s="3"/>
     </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="E40" s="3"/>
       <c r="H40" s="3"/>
@@ -1122,7 +1436,7 @@
       <c r="AI40" s="3"/>
       <c r="AL40" s="3"/>
     </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <f>SUM(B27:B40)</f>
         <v>0</v>
@@ -1198,7 +1512,7 @@
       </c>
       <c r="AM41" s="1"/>
     </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C42">
         <f>B41-C41</f>
         <v>0</v>
@@ -1252,7 +1566,1281 @@
         <v>0</v>
       </c>
     </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C49" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50">
+        <f>SUM(E47:E49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="J53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54">
+        <f>E42</f>
+        <v>0</v>
+      </c>
+      <c r="G54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J54" s="3">
+        <f>R42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="3">
+        <f>I42</f>
+        <v>0</v>
+      </c>
+      <c r="G55" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" s="3">
+        <f>AA42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56">
+        <f>AC42</f>
+        <v>0</v>
+      </c>
+      <c r="G56" t="s">
+        <v>26</v>
+      </c>
+      <c r="J56" s="3">
+        <f>L42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="3">
+        <f>AM42</f>
+        <v>0</v>
+      </c>
+      <c r="G57" t="s">
+        <v>0</v>
+      </c>
+      <c r="J57" s="3">
+        <f>C42</f>
+        <v>0</v>
+      </c>
+      <c r="K57" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="3">
+        <f>U42</f>
+        <v>0</v>
+      </c>
+      <c r="G58" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" s="3"/>
+      <c r="K58">
+        <f>W42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="3">
+        <f>AJ42</f>
+        <v>0</v>
+      </c>
+      <c r="G59" t="s">
+        <v>23</v>
+      </c>
+      <c r="J59" s="3"/>
+      <c r="K59">
+        <f>AF42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D60" s="3"/>
+      <c r="G60" t="s">
+        <v>28</v>
+      </c>
+      <c r="J60" s="3"/>
+      <c r="K60">
+        <f>N42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D61" s="2">
+        <f>SUM(D54:D60)</f>
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <f>SUM(E54:E60)</f>
+        <v>0</v>
+      </c>
+      <c r="J61" s="2">
+        <f>SUM(J54:J60)</f>
+        <v>0</v>
+      </c>
+      <c r="K61" s="1">
+        <f>SUM(K54:K60)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="7">
+        <f>E61-D61</f>
+        <v>0</v>
+      </c>
+      <c r="E62" s="8"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="4">
+        <f>D62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <f>D61+D62</f>
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <f>E61+E62</f>
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <f>J61+J62</f>
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <f>K61+K62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="E68" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="1"/>
+      <c r="H68" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68" s="1"/>
+      <c r="K68" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L68" s="1"/>
+      <c r="N68" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O68" s="1"/>
+      <c r="Q68" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R68" s="1"/>
+      <c r="T68" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U68" s="1"/>
+      <c r="W68" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X68" s="1"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="H69" s="9"/>
+      <c r="K69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="Q69" s="3"/>
+      <c r="T69" s="3"/>
+      <c r="W69" s="3"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="W70" s="3"/>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="W71" s="3"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>11</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="Q72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="W72" s="3"/>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="T73" s="3"/>
+      <c r="W73" s="3"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="Q74" s="3"/>
+      <c r="T74" s="3"/>
+      <c r="W74" s="3"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="Q75" s="3"/>
+      <c r="T75" s="3"/>
+      <c r="W75" s="3"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>15</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="Q76" s="3"/>
+      <c r="T76" s="3"/>
+      <c r="W76" s="3"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="T77" s="3"/>
+      <c r="W77" s="3"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="W78" s="3"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="T79" s="3"/>
+      <c r="W79" s="3"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="T80" s="3"/>
+      <c r="W80" s="3"/>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="T81" s="3"/>
+      <c r="W81" s="3"/>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>56</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="Q82" s="3"/>
+      <c r="T82" s="3"/>
+      <c r="W82" s="3"/>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B83" s="2">
+        <f>SUM(B69:B82)</f>
+        <v>0</v>
+      </c>
+      <c r="C83" s="1">
+        <f>SUM(C69:C82)</f>
+        <v>0</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" s="1">
+        <f>SUM(F69:F82)</f>
+        <v>0</v>
+      </c>
+      <c r="H83" s="2">
+        <f>SUM(H70:H82)</f>
+        <v>0</v>
+      </c>
+      <c r="I83" s="1"/>
+      <c r="K83" s="2">
+        <f>SUM(K69:K82)</f>
+        <v>0</v>
+      </c>
+      <c r="L83" s="1">
+        <f>SUM(L69:L82)</f>
+        <v>0</v>
+      </c>
+      <c r="N83" s="2">
+        <f>SUM(N69:N82)</f>
+        <v>0</v>
+      </c>
+      <c r="O83" s="1">
+        <f>SUM(O70:O82)</f>
+        <v>0</v>
+      </c>
+      <c r="Q83" s="2">
+        <f>SUM(Q69:Q82)</f>
+        <v>0</v>
+      </c>
+      <c r="R83" s="1">
+        <f>SUM(R69:R82)</f>
+        <v>0</v>
+      </c>
+      <c r="T83" s="2">
+        <f>SUM(T69:T82)</f>
+        <v>0</v>
+      </c>
+      <c r="U83" s="1"/>
+      <c r="W83" s="2">
+        <f>SUM(W69:W82)</f>
+        <v>0</v>
+      </c>
+      <c r="X83" s="1"/>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <f>B83-C83</f>
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <f>F83</f>
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <f>H83</f>
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <f>K83-L83</f>
+        <v>0</v>
+      </c>
+      <c r="N84">
+        <f>O83-N83</f>
+        <v>0</v>
+      </c>
+      <c r="R84">
+        <f>Q83-R83</f>
+        <v>0</v>
+      </c>
+      <c r="U84">
+        <f>T83</f>
+        <v>0</v>
+      </c>
+      <c r="X84">
+        <f>W83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B86" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="E86" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="1"/>
+      <c r="H86" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I86" s="1"/>
+      <c r="K86" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L86" s="1"/>
+      <c r="N86" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O86" s="1"/>
+      <c r="Q86" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R86" s="1"/>
+      <c r="T86" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U86" s="1"/>
+      <c r="W86" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X86" s="1"/>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="T87" s="3"/>
+      <c r="W87" s="3"/>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="Q88" s="3"/>
+      <c r="T88" s="3"/>
+      <c r="W88" s="3"/>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="Q89" s="3"/>
+      <c r="T89" s="3"/>
+      <c r="W89" s="3"/>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>11</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="W90" s="3"/>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="T91" s="3"/>
+      <c r="W91" s="3"/>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>13</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="Q92" s="3"/>
+      <c r="T92" s="3"/>
+      <c r="W92" s="3"/>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="N93" s="3"/>
+      <c r="Q93" s="3"/>
+      <c r="T93" s="3"/>
+      <c r="W93" s="3"/>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>15</v>
+      </c>
+      <c r="B94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="N94" s="3"/>
+      <c r="Q94" s="3"/>
+      <c r="T94" s="3"/>
+      <c r="W94" s="3"/>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="N95" s="3"/>
+      <c r="Q95" s="3"/>
+      <c r="T95" s="3"/>
+      <c r="W95" s="3"/>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="N96" s="3"/>
+      <c r="Q96" s="3"/>
+      <c r="T96" s="3"/>
+      <c r="W96" s="3"/>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="N97" s="3"/>
+      <c r="Q97" s="3"/>
+      <c r="T97" s="3"/>
+      <c r="W97" s="3"/>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="N98" s="3"/>
+      <c r="Q98" s="3"/>
+      <c r="T98" s="3"/>
+      <c r="W98" s="3"/>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="N99" s="3"/>
+      <c r="Q99" s="3"/>
+      <c r="T99" s="3"/>
+      <c r="W99" s="3"/>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>56</v>
+      </c>
+      <c r="B100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="N100" s="3"/>
+      <c r="Q100" s="3"/>
+      <c r="T100" s="3"/>
+      <c r="W100" s="3"/>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B101" s="2">
+        <f>SUM(B87:B100)</f>
+        <v>0</v>
+      </c>
+      <c r="C101" s="1">
+        <f>SUM(C87:C100)</f>
+        <v>0</v>
+      </c>
+      <c r="E101" s="2">
+        <f>SUM(E87:E100)</f>
+        <v>0</v>
+      </c>
+      <c r="F101" s="1">
+        <f>SUM(F87:F100)</f>
+        <v>0</v>
+      </c>
+      <c r="H101" s="2">
+        <f>SUM(H87:H100)</f>
+        <v>0</v>
+      </c>
+      <c r="I101" s="1"/>
+      <c r="K101" s="2">
+        <f>SUM(K87:K100)</f>
+        <v>0</v>
+      </c>
+      <c r="L101" s="1"/>
+      <c r="N101" s="2">
+        <f>SUM(N87:N100)</f>
+        <v>0</v>
+      </c>
+      <c r="O101" s="1"/>
+      <c r="Q101" s="2">
+        <f>SUM(Q87:Q100)</f>
+        <v>0</v>
+      </c>
+      <c r="R101" s="1">
+        <f>SUM(R87:R100)</f>
+        <v>0</v>
+      </c>
+      <c r="T101" s="2">
+        <f>SUM(T87:T100)</f>
+        <v>0</v>
+      </c>
+      <c r="U101" s="1"/>
+      <c r="W101" s="2"/>
+      <c r="X101" s="1">
+        <f>SUM(X87:X100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <f>B101-C101</f>
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <f>F101-E101</f>
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <f>H101</f>
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <f>K101</f>
+        <v>0</v>
+      </c>
+      <c r="O102">
+        <f>N101</f>
+        <v>0</v>
+      </c>
+      <c r="R102">
+        <f>Q101-R101</f>
+        <v>0</v>
+      </c>
+      <c r="U102">
+        <f>T101</f>
+        <v>0</v>
+      </c>
+      <c r="W102">
+        <f>X101</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" t="s">
+        <v>57</v>
+      </c>
+      <c r="K104" t="s">
+        <v>74</v>
+      </c>
+      <c r="M104" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="N104" s="11"/>
+      <c r="O104" s="11"/>
+      <c r="P104" s="11"/>
+      <c r="Q104" s="9"/>
+      <c r="R104" s="16">
+        <f xml:space="preserve"> E109</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>55</v>
+      </c>
+      <c r="M105" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q105" s="3"/>
+      <c r="R105" s="3"/>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M106" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q106" s="3"/>
+      <c r="R106" s="3"/>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M107" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q107" s="3"/>
+      <c r="R107" s="16">
+        <f>D110</f>
+        <v>0</v>
+      </c>
+      <c r="S107" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" s="1"/>
+      <c r="J108" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K108" s="1"/>
+      <c r="M108" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q108" s="3"/>
+      <c r="R108" s="16">
+        <f>-E111</f>
+        <v>0</v>
+      </c>
+      <c r="S108" s="5"/>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" s="3"/>
+      <c r="E109">
+        <f>E84</f>
+        <v>0</v>
+      </c>
+      <c r="G109" t="s">
+        <v>18</v>
+      </c>
+      <c r="J109" s="3">
+        <f>R84</f>
+        <v>0</v>
+      </c>
+      <c r="M109" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q109" s="3"/>
+      <c r="R109" s="3"/>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>25</v>
+      </c>
+      <c r="D110" s="3">
+        <f>I84</f>
+        <v>0</v>
+      </c>
+      <c r="G110" t="s">
+        <v>21</v>
+      </c>
+      <c r="J110" s="3">
+        <f>U102</f>
+        <v>0</v>
+      </c>
+      <c r="M110" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q110" s="3"/>
+      <c r="R110" s="3"/>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>22</v>
+      </c>
+      <c r="D111" s="3"/>
+      <c r="E111">
+        <f>W102</f>
+        <v>0</v>
+      </c>
+      <c r="G111" t="s">
+        <v>58</v>
+      </c>
+      <c r="J111" s="3">
+        <f>L84+I102</f>
+        <v>0</v>
+      </c>
+      <c r="M111" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q111" s="3"/>
+      <c r="R111" s="16">
+        <f>X84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>59</v>
+      </c>
+      <c r="D112" s="3">
+        <f>X84+L102</f>
+        <v>0</v>
+      </c>
+      <c r="G112" t="s">
+        <v>0</v>
+      </c>
+      <c r="J112" s="3">
+        <f>C84</f>
+        <v>0</v>
+      </c>
+      <c r="K112" t="s">
+        <v>52</v>
+      </c>
+      <c r="M112" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q112" s="3"/>
+      <c r="R112" s="3"/>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113" s="3">
+        <f>U84</f>
+        <v>0</v>
+      </c>
+      <c r="G113" t="s">
+        <v>40</v>
+      </c>
+      <c r="J113" s="3">
+        <f>C102</f>
+        <v>0</v>
+      </c>
+      <c r="M113" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q113" s="3"/>
+      <c r="R113" s="16">
+        <f>L102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>60</v>
+      </c>
+      <c r="D114" s="3">
+        <f>R102+O102</f>
+        <v>0</v>
+      </c>
+      <c r="G114" t="s">
+        <v>20</v>
+      </c>
+      <c r="J114" s="3"/>
+      <c r="K114">
+        <f>E102</f>
+        <v>0</v>
+      </c>
+      <c r="M114" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q114" s="3"/>
+      <c r="R114" s="15"/>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D115" s="3"/>
+      <c r="G115" t="s">
+        <v>28</v>
+      </c>
+      <c r="J115" s="3"/>
+      <c r="K115">
+        <f>N84</f>
+        <v>0</v>
+      </c>
+      <c r="M115" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q115" s="3"/>
+      <c r="R115" s="15">
+        <f>D113</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D116" s="2">
+        <f>SUM(D109:D115)</f>
+        <v>0</v>
+      </c>
+      <c r="E116" s="1">
+        <f>SUM(E109:E115)</f>
+        <v>0</v>
+      </c>
+      <c r="J116" s="2">
+        <f>SUM(J109:J115)</f>
+        <v>0</v>
+      </c>
+      <c r="K116" s="1">
+        <f>SUM(K109:K115)</f>
+        <v>0</v>
+      </c>
+      <c r="M116" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q116" s="3"/>
+      <c r="R116" s="16"/>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>53</v>
+      </c>
+      <c r="D117" s="7">
+        <f>E116-D116</f>
+        <v>0</v>
+      </c>
+      <c r="E117" s="8"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="4">
+        <f>D117</f>
+        <v>0</v>
+      </c>
+      <c r="M117" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q117" s="3"/>
+      <c r="R117" s="15">
+        <f>D114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <f>D116+D117</f>
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <f>E116+E117</f>
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <f>J116+J117</f>
+        <v>0</v>
+      </c>
+      <c r="K118">
+        <f>K116+K117</f>
+        <v>0</v>
+      </c>
+      <c r="M118" s="12"/>
+      <c r="Q118" s="3"/>
+      <c r="R118" s="3"/>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L119" s="3"/>
+      <c r="M119" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="N119" s="1"/>
+      <c r="O119" s="1"/>
+      <c r="P119" s="1"/>
+      <c r="Q119" s="2"/>
+      <c r="R119" s="2">
+        <f>R104-SUM(R105:R118)</f>
+        <v>0</v>
+      </c>
+      <c r="T119" s="13"/>
+      <c r="U119" s="13"/>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L120" s="13"/>
+      <c r="M120" s="13"/>
+      <c r="N120" s="13"/>
+      <c r="O120" s="13"/>
+      <c r="P120" s="13"/>
+      <c r="Q120" s="13"/>
+      <c r="R120" s="13"/>
+      <c r="S120" s="13"/>
+      <c r="T120" s="13"/>
+      <c r="U120" s="13"/>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L121" s="13"/>
+      <c r="M121" s="13"/>
+      <c r="N121" s="13"/>
+      <c r="O121" s="13"/>
+      <c r="P121" s="13"/>
+      <c r="Q121" s="13"/>
+      <c r="R121" s="13"/>
+      <c r="S121" s="13"/>
+      <c r="T121" s="13"/>
+      <c r="U121" s="13"/>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L122" s="13"/>
+      <c r="M122" s="13"/>
+      <c r="N122" s="13"/>
+      <c r="O122" s="13"/>
+      <c r="P122" s="13"/>
+      <c r="Q122" s="13"/>
+      <c r="R122" s="13"/>
+      <c r="S122" s="13"/>
+      <c r="T122" s="13"/>
+      <c r="U122" s="13"/>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L123" s="13"/>
+      <c r="M123" s="13"/>
+      <c r="N123" s="13"/>
+      <c r="O123" s="13"/>
+      <c r="P123" s="13"/>
+      <c r="Q123" s="13"/>
+      <c r="R123" s="13"/>
+      <c r="S123" s="13"/>
+      <c r="T123" s="13"/>
+      <c r="U123" s="13"/>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L124" s="13"/>
+      <c r="M124" s="13"/>
+      <c r="N124" s="13"/>
+      <c r="O124" s="13"/>
+      <c r="P124" s="13"/>
+      <c r="Q124" s="13"/>
+      <c r="R124" s="13"/>
+      <c r="S124" s="13"/>
+      <c r="T124" s="13"/>
+      <c r="U124" s="13"/>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L125" s="13"/>
+      <c r="M125" s="13"/>
+      <c r="N125" s="13"/>
+      <c r="O125" s="13"/>
+      <c r="P125" s="13"/>
+      <c r="Q125" s="13"/>
+      <c r="R125" s="13"/>
+      <c r="S125" s="13"/>
+      <c r="T125" s="13"/>
+      <c r="U125" s="13"/>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L126" s="13"/>
+      <c r="M126" s="13"/>
+      <c r="N126" s="13"/>
+      <c r="O126" s="13"/>
+      <c r="P126" s="13"/>
+      <c r="Q126" s="13"/>
+      <c r="R126" s="13"/>
+      <c r="S126" s="13"/>
+      <c r="T126" s="13"/>
+      <c r="U126" s="13"/>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L127" s="13"/>
+      <c r="M127" s="13"/>
+      <c r="N127" s="13"/>
+      <c r="O127" s="13"/>
+      <c r="P127" s="13"/>
+      <c r="Q127" s="13"/>
+      <c r="R127" s="13"/>
+      <c r="S127" s="13"/>
+      <c r="T127" s="13"/>
+      <c r="U127" s="13"/>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L128" s="13"/>
+      <c r="M128" s="13"/>
+      <c r="N128" s="13"/>
+      <c r="O128" s="13"/>
+      <c r="P128" s="13"/>
+      <c r="Q128" s="13"/>
+      <c r="R128" s="13"/>
+      <c r="S128" s="13"/>
+      <c r="T128" s="13"/>
+      <c r="U128" s="13"/>
+    </row>
+    <row r="129" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="L129" s="13"/>
+      <c r="M129" s="13"/>
+      <c r="N129" s="13"/>
+      <c r="O129" s="13"/>
+      <c r="P129" s="13"/>
+      <c r="Q129" s="13"/>
+      <c r="R129" s="13"/>
+      <c r="S129" s="13"/>
+      <c r="T129" s="13"/>
+      <c r="U129" s="13"/>
+    </row>
+    <row r="130" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="L130" s="13"/>
+      <c r="M130" s="13"/>
+      <c r="N130" s="13"/>
+      <c r="O130" s="13"/>
+      <c r="P130" s="13"/>
+      <c r="Q130" s="13"/>
+      <c r="R130" s="13"/>
+      <c r="S130" s="13"/>
+      <c r="T130" s="13"/>
+      <c r="U130" s="13"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="17"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Harkka 5 pohja + ratkaisut
</commit_message>
<xml_diff>
--- a/harkat/harkat_pohja.xlsx
+++ b/harkat/harkat_pohja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuni-my.sharepoint.com/personal/teemu_helenius_tuni_fi/Documents/Yrityksen talous/tiiviste/harkat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="8_{89EAE0E3-53EA-4691-BDD9-A76C84E4BCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0AC4C0B4-AE07-42A8-95F7-0792B8A19800}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="8_{89EAE0E3-53EA-4691-BDD9-A76C84E4BCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{63CA3FA9-47AD-47E0-8DE1-353842D7B248}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="92">
   <si>
     <t>Kassa</t>
   </si>
@@ -265,16 +265,67 @@
   </si>
   <si>
     <t>H5</t>
+  </si>
+  <si>
+    <t>K8</t>
+  </si>
+  <si>
+    <t>K34</t>
+  </si>
+  <si>
+    <t>Vain yksi tunnusluku pitää osata laskea tentissä, sijoitetun pääoman tuotto aka ROI</t>
+  </si>
+  <si>
+    <t>Loput pitää tietää, onko hyvä, tyydyttävä vai huono tunnusluku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROI harkassa = </t>
+  </si>
+  <si>
+    <t>Viitearvoja tunnusluvuille, kaikki tyydyttäviä ja suurempi hyvä</t>
+  </si>
+  <si>
+    <t>Liiketulos</t>
+  </si>
+  <si>
+    <t>Nettotulos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick ratio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current ratio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omavaraisuusaste </t>
+  </si>
+  <si>
+    <t>ROI:n kaava =</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = ?</t>
+  </si>
+  <si>
+    <t>Myyntikate (= ?) ja käyttökate (= ?)</t>
+  </si>
+  <si>
+    <t>Huom. Löytyykö virallisesta tilinpäätöksestä nettotulosta?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -457,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -476,6 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -556,6 +608,429 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>34278</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>107876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Kuva 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4977D3A4-0F9F-44AB-9D71-33678DDCB362}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect t="14438" b="14285"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="30489525"/>
+          <a:ext cx="8568678" cy="4289351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>474051</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>42128</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3159370" cy="318036"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="Tekstiruutu 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C5BEF1-DF00-4784-804D-135B97911ADC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9618051" y="30712628"/>
+              <a:ext cx="3159370" cy="318036"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="fi-FI" sz="1100">
+                            <a:solidFill>
+                              <a:srgbClr val="836967"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="fi-FI" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>?+</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="fi-FI" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>?+? </m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="fi-FI" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>?</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="fi-FI" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="Tekstiruutu 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C5BEF1-DF00-4784-804D-135B97911ADC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9618051" y="30712628"/>
+              <a:ext cx="3159370" cy="318036"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fi-FI" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="836967"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="fi-FI" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>?+?+? </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="fi-FI" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="836967"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="fi-FI" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>?</a:t>
+              </a:r>
+              <a:endParaRPr lang="fi-FI" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>445475</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>4027</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3291255" cy="611435"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="Tekstiruutu 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{870337A0-6CF6-45BD-BF8F-11BBB4E196D6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9589475" y="31627027"/>
+              <a:ext cx="3291255" cy="611435"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="fi-FI" sz="1400">
+                            <a:solidFill>
+                              <a:srgbClr val="836967"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num/>
+                      <m:den>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="fi-FI" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="fi-FI" sz="1400" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e/>
+                            </m:d>
+                            <m:r>
+                              <a:rPr lang="fi-FI" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>+</m:t>
+                            </m:r>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="fi-FI" sz="1400" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e/>
+                            </m:d>
+                          </m:num>
+                          <m:den/>
+                        </m:f>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="fi-FI" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="Tekstiruutu 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{870337A0-6CF6-45BD-BF8F-11BBB4E196D6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9589475" y="31627027"/>
+              <a:ext cx="3291255" cy="611435"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fi-FI" sz="1400" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="836967"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>/(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="fi-FI" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="836967"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>((┤)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="fi-FI" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>+(┤))/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="fi-FI" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="836967"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:endParaRPr lang="fi-FI" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -822,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM159"/>
+  <dimension ref="A1:AM178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="L155" sqref="L155"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S176" sqref="S176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,12 +3306,94 @@
       <c r="T130" s="13"/>
       <c r="U130" s="13"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="17"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>76</v>
+      </c>
+      <c r="C159" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D159" t="s">
+        <v>90</v>
+      </c>
+      <c r="O159" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P159" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C160" s="5"/>
+      <c r="D160" t="s">
+        <v>91</v>
+      </c>
+      <c r="O160" s="5"/>
+      <c r="P160" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="163" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O163" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="168" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="171" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="Q171" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="173" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O173" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="174" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O174" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q174" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="175" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O175" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q175" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="176" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O176" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q176" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="177" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O177" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q177" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="178" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O178" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q178" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Johdon laskentatoimen harkat 1-3
</commit_message>
<xml_diff>
--- a/harkat/harkat_pohja.xlsx
+++ b/harkat/harkat_pohja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuni-my.sharepoint.com/personal/teemu_helenius_tuni_fi/Documents/Yrityksen talous/tiiviste/harkat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="8_{89EAE0E3-53EA-4691-BDD9-A76C84E4BCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{63CA3FA9-47AD-47E0-8DE1-353842D7B248}"/>
+  <xr:revisionPtr revIDLastSave="338" documentId="8_{89EAE0E3-53EA-4691-BDD9-A76C84E4BCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0E8FDB5D-65CE-41DE-B894-719A5F18B4F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
   <si>
     <t>Kassa</t>
   </si>
@@ -310,13 +310,115 @@
   </si>
   <si>
     <t>Huom. Löytyykö virallisesta tilinpäätöksestä nettotulosta?</t>
+  </si>
+  <si>
+    <t>Johdon laskentatoimi</t>
+  </si>
+  <si>
+    <t>a) Laske yrityksen katetuottoprosentti, kriittisen pisteen myynti ja varmuusmarginaali</t>
+  </si>
+  <si>
+    <t>K9</t>
+  </si>
+  <si>
+    <t>Katetuottoprosentti =</t>
+  </si>
+  <si>
+    <t>Kriittinen piste =</t>
+  </si>
+  <si>
+    <t>Varmuusmarginaali =</t>
+  </si>
+  <si>
+    <t>Yritys</t>
+  </si>
+  <si>
+    <t>Tuote 1</t>
+  </si>
+  <si>
+    <t>Tuote 2</t>
+  </si>
+  <si>
+    <t>Tuote 3</t>
+  </si>
+  <si>
+    <t>välittömät</t>
+  </si>
+  <si>
+    <t>Kiinteät erilliskustannukset</t>
+  </si>
+  <si>
+    <t>Tuotteen erilliskate</t>
+  </si>
+  <si>
+    <t>välilliset</t>
+  </si>
+  <si>
+    <t>Kiinteät yhteiskustannukset</t>
+  </si>
+  <si>
+    <t>% = ?</t>
+  </si>
+  <si>
+    <t>b) Katetuotto 20%. Hintojen laskeminen 10%. Uusi katetuottto prosentti = ?, katetuotto prosentti laskee ?  = ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Erikoisliikkeen keskimääräinen katetuottoprosentti laskee = ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Gigamyynnin keskimääräinen katetuottoprosentti laskee = ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Erikoisliikkeen tulos = ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     (Giganmyynnin tulos kuvitteellisilla arvoilla = 3%-?% = ?%)</t>
+  </si>
+  <si>
+    <t>K12</t>
+  </si>
+  <si>
+    <t>Vuosi</t>
+  </si>
+  <si>
+    <t>Poistoprosentti</t>
+  </si>
+  <si>
+    <t>Poisto</t>
+  </si>
+  <si>
+    <t>Poistamaton osuus</t>
+  </si>
+  <si>
+    <t>d)</t>
+  </si>
+  <si>
+    <t>Annuiteetti</t>
+  </si>
+  <si>
+    <t>Korko</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>Annuiteettilaina tentissä, sama menetelmä</t>
+  </si>
+  <si>
+    <t>Annuiteettitekijä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annuiteetti </t>
+  </si>
+  <si>
+    <t>Täytä annuiteettitekijä</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,8 +432,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +456,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -528,6 +643,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -556,7 +679,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:colOff>186772</xdr:colOff>
       <xdr:row>154</xdr:row>
       <xdr:rowOff>182841</xdr:rowOff>
     </xdr:to>
@@ -616,8 +739,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>34278</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>481539</xdr:colOff>
       <xdr:row>182</xdr:row>
       <xdr:rowOff>107876</xdr:rowOff>
     </xdr:to>
@@ -659,8 +782,8 @@
       <xdr:rowOff>42128</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3159370" cy="318036"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="Tekstiruutu 8">
@@ -702,6 +825,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -711,7 +835,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="fi-FI" sz="1100">
+                          <a:rPr lang="fi-FI" sz="1100" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -750,7 +874,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="Tekstiruutu 8">
@@ -838,8 +962,8 @@
       <xdr:rowOff>4027</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3291255" cy="611435"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="Tekstiruutu 9">
@@ -881,6 +1005,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -890,7 +1015,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="fi-FI" sz="1400">
+                          <a:rPr lang="fi-FI" sz="1400" i="1">
                             <a:solidFill>
                               <a:srgbClr val="836967"/>
                             </a:solidFill>
@@ -948,7 +1073,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="Tekstiruutu 9">
@@ -1031,6 +1156,492 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>439616</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>4424</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Kuva 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{834F9704-3C28-4563-BCDD-9983DD33A435}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="624700" y="35939514"/>
+          <a:ext cx="4255031" cy="1520141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7323</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>7328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>424961</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>189318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Kuva 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE29148D-9FA8-4466-A332-F4FEE533EE2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5663708" y="36129059"/>
+          <a:ext cx="5282715" cy="1324990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>21983</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>111178</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>57671</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Kuva 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBFFA057-59DD-4818-8B1A-D37CB0CE0637}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11151579" y="36114404"/>
+          <a:ext cx="4346137" cy="2160498"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>439616</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>4424</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Kuva 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E41AC90C-E5F5-47F1-B54B-F6DBC545C10F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="626165" y="35936583"/>
+          <a:ext cx="4271151" cy="1520141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7323</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>7328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>424961</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>189318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Kuva 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5178EDC9-8FEE-45BC-95E8-9FD7C6426FDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5493723" y="36126128"/>
+          <a:ext cx="5294438" cy="1324990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>21984</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>573821</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Kuva 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70EAB66C-0025-4B14-AA31-1286A6C0F8D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10994784" y="36111473"/>
+          <a:ext cx="4209437" cy="2088173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>643895</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>14654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>188653</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Kuva 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{941BBD80-656F-4B3C-96B1-F468686D4459}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect b="34196"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1252030" y="37850885"/>
+          <a:ext cx="3810874" cy="745499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>6568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>428790</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>6569</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Kuva 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DDCF333-1215-4F4C-B975-EC8F01FC87A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609601" y="39935368"/>
+          <a:ext cx="4276889" cy="2286001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1297,13 +1908,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM178"/>
+  <dimension ref="A1:AM247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S176" sqref="S176"/>
+    <sheetView tabSelected="1" topLeftCell="A227" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N248" sqref="N248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="9.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
@@ -3380,7 +3994,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="177" spans="15:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O177" t="s">
         <v>86</v>
       </c>
@@ -3388,12 +4002,475 @@
         <v>89</v>
       </c>
     </row>
-    <row r="178" spans="15:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O178" t="s">
         <v>87</v>
       </c>
       <c r="Q178" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" ht="39" x14ac:dyDescent="0.6">
+      <c r="A186" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A188" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I188" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J188" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J197" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J199" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>31</v>
+      </c>
+      <c r="B201" s="8"/>
+      <c r="C201" s="4"/>
+      <c r="D201" s="7"/>
+      <c r="E201" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F201" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G201" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H201" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>102</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C202" s="4"/>
+      <c r="D202" s="7"/>
+      <c r="E202" s="7">
+        <f>SUM(F202:H202)</f>
+        <v>0</v>
+      </c>
+      <c r="F202" s="16"/>
+      <c r="G202" s="16"/>
+      <c r="H202" s="7"/>
+    </row>
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B203" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C203" s="4"/>
+      <c r="D203" s="7"/>
+      <c r="E203" s="7">
+        <f>SUM(F203:H203)</f>
+        <v>0</v>
+      </c>
+      <c r="F203" s="16"/>
+      <c r="G203" s="16"/>
+      <c r="H203" s="16"/>
+      <c r="J203" t="s">
+        <v>97</v>
+      </c>
+      <c r="S203" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>105</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C204" s="4"/>
+      <c r="D204" s="7"/>
+      <c r="E204" s="16"/>
+      <c r="F204" s="11"/>
+      <c r="G204" s="11"/>
+    </row>
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B205" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C205" s="1"/>
+      <c r="D205" s="2"/>
+      <c r="E205" s="16"/>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A208" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I209" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I210" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I212" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I214" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I215" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I217" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I218" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A223" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B223" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="225" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>4</v>
+      </c>
+      <c r="C225" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D225" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E225" s="16"/>
+      <c r="F225" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G225" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H225" s="16"/>
+    </row>
+    <row r="226" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C226" s="16">
+        <v>1</v>
+      </c>
+      <c r="D226" s="1"/>
+      <c r="E226" s="7"/>
+      <c r="F226" s="22"/>
+      <c r="G226" s="8"/>
+      <c r="H226" s="23"/>
+    </row>
+    <row r="227" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C227" s="16">
+        <v>2</v>
+      </c>
+      <c r="D227" s="1"/>
+      <c r="E227" s="7"/>
+      <c r="F227" s="22"/>
+      <c r="G227" s="8"/>
+      <c r="H227" s="23"/>
+    </row>
+    <row r="228" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C228" s="16">
+        <v>3</v>
+      </c>
+      <c r="D228" s="1"/>
+      <c r="E228" s="7"/>
+      <c r="F228" s="22"/>
+      <c r="G228" s="8"/>
+      <c r="H228" s="23"/>
+    </row>
+    <row r="229" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C229" s="16">
+        <v>4</v>
+      </c>
+      <c r="D229" s="1"/>
+      <c r="E229" s="7"/>
+      <c r="F229" s="22"/>
+      <c r="G229" s="8"/>
+      <c r="H229" s="7"/>
+    </row>
+    <row r="231" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
+        <v>31</v>
+      </c>
+      <c r="C231" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D231" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E231" s="16"/>
+      <c r="F231" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G231" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H231" s="16"/>
+    </row>
+    <row r="232" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C232" s="16">
+        <v>1</v>
+      </c>
+      <c r="D232" s="1"/>
+      <c r="E232" s="7"/>
+      <c r="F232" s="22"/>
+      <c r="G232" s="8"/>
+      <c r="H232" s="23">
+        <f>60000-F232</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="233" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C233" s="16">
+        <v>2</v>
+      </c>
+      <c r="D233" s="1"/>
+      <c r="E233" s="7"/>
+      <c r="F233" s="22"/>
+      <c r="G233" s="8"/>
+      <c r="H233" s="23">
+        <f>H232-F233</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="234" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C234" s="16">
+        <v>3</v>
+      </c>
+      <c r="D234" s="1"/>
+      <c r="E234" s="7"/>
+      <c r="F234" s="22"/>
+      <c r="G234" s="8"/>
+      <c r="H234" s="23">
+        <f>H233-F234</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="235" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C235" s="16">
+        <v>4</v>
+      </c>
+      <c r="D235" s="1"/>
+      <c r="E235" s="7"/>
+      <c r="F235" s="22"/>
+      <c r="G235" s="8"/>
+      <c r="H235" s="23">
+        <f t="shared" ref="H234:H235" si="0">H234-F235</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="237" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
+        <v>5</v>
+      </c>
+      <c r="C237" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D237" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E237" s="16"/>
+      <c r="F237" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G237" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H237" s="16"/>
+    </row>
+    <row r="238" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C238" s="16">
+        <v>1</v>
+      </c>
+      <c r="D238" s="1"/>
+      <c r="E238" s="7"/>
+      <c r="F238" s="22"/>
+      <c r="G238" s="8"/>
+      <c r="H238" s="23">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="239" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C239" s="16">
+        <v>2</v>
+      </c>
+      <c r="D239" s="1"/>
+      <c r="E239" s="7"/>
+      <c r="F239" s="22"/>
+      <c r="G239" s="8"/>
+      <c r="H239" s="23">
+        <f>H238-F239</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="240" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C240" s="16">
+        <v>3</v>
+      </c>
+      <c r="D240" s="1"/>
+      <c r="E240" s="7"/>
+      <c r="F240" s="22"/>
+      <c r="G240" s="8"/>
+      <c r="H240" s="23">
+        <f>H239-F240</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="241" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C241" s="16">
+        <v>4</v>
+      </c>
+      <c r="D241" s="1"/>
+      <c r="E241" s="7"/>
+      <c r="F241" s="22"/>
+      <c r="G241" s="8"/>
+      <c r="H241" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>118</v>
+      </c>
+      <c r="C243" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D243" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E243" s="16"/>
+      <c r="F243" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G243" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H243" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="I243" s="16"/>
+      <c r="K243" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L243" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="244" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C244" s="16">
+        <v>1</v>
+      </c>
+      <c r="D244" s="1"/>
+      <c r="E244" s="24">
+        <f>M246</f>
+        <v>0</v>
+      </c>
+      <c r="F244" s="22"/>
+      <c r="G244" s="22"/>
+      <c r="H244" s="25"/>
+      <c r="I244" s="23">
+        <f>60000-G244</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="245" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C245" s="16">
+        <v>2</v>
+      </c>
+      <c r="D245" s="1"/>
+      <c r="E245" s="7">
+        <f>M246</f>
+        <v>0</v>
+      </c>
+      <c r="F245" s="22"/>
+      <c r="G245" s="22"/>
+      <c r="H245" s="8"/>
+      <c r="I245" s="23">
+        <f>I244-G245</f>
+        <v>60000</v>
+      </c>
+      <c r="K245" t="s">
+        <v>123</v>
+      </c>
+      <c r="M245">
+        <v>0</v>
+      </c>
+      <c r="N245" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="246" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C246" s="16">
+        <v>3</v>
+      </c>
+      <c r="D246" s="1"/>
+      <c r="E246" s="7">
+        <f>M246</f>
+        <v>0</v>
+      </c>
+      <c r="F246" s="22"/>
+      <c r="G246" s="22"/>
+      <c r="H246" s="8"/>
+      <c r="I246" s="23">
+        <f t="shared" ref="I246:I247" si="1">I245-G246</f>
+        <v>60000</v>
+      </c>
+      <c r="K246" t="s">
+        <v>124</v>
+      </c>
+      <c r="M246" s="26">
+        <f>60000*M245</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C247" s="16">
+        <v>4</v>
+      </c>
+      <c r="D247" s="1"/>
+      <c r="E247" s="7">
+        <f>M246</f>
+        <v>0</v>
+      </c>
+      <c r="F247" s="22"/>
+      <c r="G247" s="22"/>
+      <c r="H247" s="8"/>
+      <c r="I247" s="23">
+        <f>I246-G247</f>
+        <v>60000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Loput harkat, kuvat omaan kansioon
</commit_message>
<xml_diff>
--- a/harkat/harkat_pohja.xlsx
+++ b/harkat/harkat_pohja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuni-my.sharepoint.com/personal/teemu_helenius_tuni_fi/Documents/Yrityksen talous/tiiviste/harkat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="338" documentId="8_{89EAE0E3-53EA-4691-BDD9-A76C84E4BCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0E8FDB5D-65CE-41DE-B894-719A5F18B4F7}"/>
+  <xr:revisionPtr revIDLastSave="364" documentId="8_{89EAE0E3-53EA-4691-BDD9-A76C84E4BCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8BBB1364-B037-4E59-800F-014C3061C5D8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="189">
   <si>
     <t>Kassa</t>
   </si>
@@ -412,6 +412,195 @@
   </si>
   <si>
     <t>Täytä annuiteettitekijä</t>
+  </si>
+  <si>
+    <t>K11</t>
+  </si>
+  <si>
+    <t>FIFO</t>
+  </si>
+  <si>
+    <t>LIFO</t>
+  </si>
+  <si>
+    <t>Jatkuvana</t>
+  </si>
+  <si>
+    <t>Ajanjaksoittain</t>
+  </si>
+  <si>
+    <t>Keskihinnan menetelmä</t>
+  </si>
+  <si>
+    <t>Alkuvarasto</t>
+  </si>
+  <si>
+    <t>300 kpl</t>
+  </si>
+  <si>
+    <t>5,5€/kpl</t>
+  </si>
+  <si>
+    <t>Käytön kustannus</t>
+  </si>
+  <si>
+    <t>Käyttö</t>
+  </si>
+  <si>
+    <t>200 kpl</t>
+  </si>
+  <si>
+    <t>Loppuvaraston arvo</t>
+  </si>
+  <si>
+    <t>Ka. Hinta=</t>
+  </si>
+  <si>
+    <t>Saapunut</t>
+  </si>
+  <si>
+    <t>500 kpl</t>
+  </si>
+  <si>
+    <t>7€/kpl</t>
+  </si>
+  <si>
+    <t>Käytön hintaero</t>
+  </si>
+  <si>
+    <t>350 kpl</t>
+  </si>
+  <si>
+    <t>Loppuvarasto</t>
+  </si>
+  <si>
+    <t>250 kpl</t>
+  </si>
+  <si>
+    <t>Päivänhintamenetelmä</t>
+  </si>
+  <si>
+    <t>Vakio- eli standardihinta</t>
+  </si>
+  <si>
+    <t>6€/kpl</t>
+  </si>
+  <si>
+    <t>e)</t>
+  </si>
+  <si>
+    <t>K16</t>
+  </si>
+  <si>
+    <t>K17</t>
+  </si>
+  <si>
+    <t>Välittömät kustannukset</t>
+  </si>
+  <si>
+    <t>Valmistus</t>
+  </si>
+  <si>
+    <t>Hallinto</t>
+  </si>
+  <si>
+    <t>raaka-aineet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>palkat</t>
+  </si>
+  <si>
+    <t>Välilliset kustannukset</t>
+  </si>
+  <si>
+    <t>muutuvat</t>
+  </si>
+  <si>
+    <t>kiinteät</t>
+  </si>
+  <si>
+    <t>YK-lisien perusteet</t>
+  </si>
+  <si>
+    <t>Minimi</t>
+  </si>
+  <si>
+    <t>Keskimääräis</t>
+  </si>
+  <si>
+    <t>Normaali</t>
+  </si>
+  <si>
+    <t>YK-lisät</t>
+  </si>
+  <si>
+    <t>Välittömät raaka-aine kustannukset</t>
+  </si>
+  <si>
+    <t>Minimikalkyyli</t>
+  </si>
+  <si>
+    <t>Raaka-ainelisät</t>
+  </si>
+  <si>
+    <t>Keskimääräiskalkyyli</t>
+  </si>
+  <si>
+    <t>Välittömät palkat</t>
+  </si>
+  <si>
+    <t>Normaalikalkyyli</t>
+  </si>
+  <si>
+    <t>Valmistuslisä</t>
+  </si>
+  <si>
+    <t>Valmistusarvo</t>
+  </si>
+  <si>
+    <t>hallinnon lisä</t>
+  </si>
+  <si>
+    <t>Omakustannusarvo</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raaka-aine </t>
+  </si>
+  <si>
+    <t>tavoite</t>
+  </si>
+  <si>
+    <t>toteutunut</t>
+  </si>
+  <si>
+    <t>Työ</t>
+  </si>
+  <si>
+    <t>Yksikköhinta €/kg</t>
+  </si>
+  <si>
+    <t>Yksikköhinta €/h</t>
+  </si>
+  <si>
+    <t>Käyttö kg/kpl</t>
+  </si>
+  <si>
+    <t>Käyttö h/kpl</t>
+  </si>
+  <si>
+    <t>Hintaero €</t>
+  </si>
+  <si>
+    <t>Määräero €</t>
+  </si>
+  <si>
+    <t>K19</t>
   </si>
 </sst>
 </file>
@@ -623,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -651,6 +840,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -1622,8 +1820,130 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609601" y="39935368"/>
-          <a:ext cx="4276889" cy="2286001"/>
+          <a:off x="608136" y="39938299"/>
+          <a:ext cx="4260769" cy="2286001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>21978</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>36636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>422762</xdr:colOff>
+      <xdr:row>269</xdr:row>
+      <xdr:rowOff>155454</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Kuva 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38307FC1-4EF2-4053-A8BD-7D772DA461A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="631578" y="50252436"/>
+          <a:ext cx="4248884" cy="1452318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>87922</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>540236</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Kuva 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F61D2196-DFA0-4171-B4BD-05517A0ACD95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="631581" y="54113722"/>
+          <a:ext cx="3109055" cy="1436079"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1908,10 +2228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM247"/>
+  <dimension ref="A1:AM289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N248" sqref="N248"/>
+    <sheetView tabSelected="1" topLeftCell="A271" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C282" sqref="C282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4288,7 +4608,7 @@
       <c r="F235" s="22"/>
       <c r="G235" s="8"/>
       <c r="H235" s="23">
-        <f t="shared" ref="H234:H235" si="0">H234-F235</f>
+        <f t="shared" ref="H235" si="0">H234-F235</f>
         <v>60000</v>
       </c>
     </row>
@@ -4349,7 +4669,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="241" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C241" s="16">
         <v>4</v>
       </c>
@@ -4361,7 +4681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
         <v>118</v>
       </c>
@@ -4389,7 +4709,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="244" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C244" s="16">
         <v>1</v>
       </c>
@@ -4406,7 +4726,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="245" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C245" s="16">
         <v>2</v>
       </c>
@@ -4432,7 +4752,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="246" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C246" s="16">
         <v>3</v>
       </c>
@@ -4445,7 +4765,7 @@
       <c r="G246" s="22"/>
       <c r="H246" s="8"/>
       <c r="I246" s="23">
-        <f t="shared" ref="I246:I247" si="1">I245-G246</f>
+        <f t="shared" ref="I246" si="1">I245-G246</f>
         <v>60000</v>
       </c>
       <c r="K246" t="s">
@@ -4456,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C247" s="16">
         <v>4</v>
       </c>
@@ -4473,6 +4793,671 @@
         <v>60000</v>
       </c>
     </row>
+    <row r="251" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A251" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I251" t="s">
+        <v>127</v>
+      </c>
+      <c r="M251" t="s">
+        <v>128</v>
+      </c>
+      <c r="O251" t="s">
+        <v>129</v>
+      </c>
+      <c r="P251" t="s">
+        <v>130</v>
+      </c>
+      <c r="R251" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="252" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C252" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D252" s="16"/>
+      <c r="E252" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F252" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H252" t="s">
+        <v>4</v>
+      </c>
+      <c r="I252" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="J252" s="7"/>
+      <c r="K252" s="16">
+        <f>300*5.5+250*7</f>
+        <v>3400</v>
+      </c>
+      <c r="L252" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="M252" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="N252" s="7"/>
+      <c r="O252" s="16">
+        <f>200*5.5+350*7</f>
+        <v>3550</v>
+      </c>
+      <c r="P252" s="16">
+        <f>500*7+50*5.5</f>
+        <v>3775</v>
+      </c>
+      <c r="R252" t="s">
+        <v>5</v>
+      </c>
+      <c r="U252" t="s">
+        <v>129</v>
+      </c>
+      <c r="V252" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="253" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C253" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D253" s="7"/>
+      <c r="E253" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F253" s="16"/>
+      <c r="I253" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J253" s="2"/>
+      <c r="K253" s="15">
+        <f>250*7</f>
+        <v>1750</v>
+      </c>
+      <c r="M253" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="N253" s="2"/>
+      <c r="O253" s="15">
+        <f>100*5.5+150*7</f>
+        <v>1600</v>
+      </c>
+      <c r="P253" s="16">
+        <f>250*5.5</f>
+        <v>1375</v>
+      </c>
+      <c r="V253" t="s">
+        <v>139</v>
+      </c>
+      <c r="W253">
+        <f>(300*5.5+500*7)/800</f>
+        <v>6.4375</v>
+      </c>
+    </row>
+    <row r="254" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C254" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D254" s="7"/>
+      <c r="E254" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F254" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="M254" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="N254" s="7"/>
+      <c r="O254" s="16">
+        <f>O252-K252</f>
+        <v>150</v>
+      </c>
+      <c r="P254" s="16">
+        <f>P252-K252</f>
+        <v>375</v>
+      </c>
+      <c r="S254" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="T254" s="7"/>
+      <c r="U254" s="16">
+        <f>200*5.5+ 350 * (100*5.5+7*500)/600</f>
+        <v>3462.5</v>
+      </c>
+      <c r="V254" s="16">
+        <f>550*W253</f>
+        <v>3540.625</v>
+      </c>
+    </row>
+    <row r="255" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C255" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D255" s="7"/>
+      <c r="E255" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F255" s="16"/>
+      <c r="S255" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="T255" s="2"/>
+      <c r="U255" s="15">
+        <f>250*(100*5.5+7*500)/600</f>
+        <v>1687.5</v>
+      </c>
+      <c r="V255" s="16">
+        <f>250*W253</f>
+        <v>1609.375</v>
+      </c>
+    </row>
+    <row r="256" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C256" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D256" s="16"/>
+      <c r="E256" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F256" s="16"/>
+      <c r="I256" t="s">
+        <v>147</v>
+      </c>
+      <c r="M256" t="s">
+        <v>148</v>
+      </c>
+      <c r="O256" t="s">
+        <v>149</v>
+      </c>
+      <c r="S256" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="T256" s="7"/>
+      <c r="U256" s="16">
+        <f>U254-K252</f>
+        <v>62.5</v>
+      </c>
+      <c r="V256" s="16">
+        <f>V254-K252</f>
+        <v>140.625</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H257" t="s">
+        <v>118</v>
+      </c>
+      <c r="I257" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="J257" s="7"/>
+      <c r="K257" s="16">
+        <f>200*5.5+350*7</f>
+        <v>3550</v>
+      </c>
+      <c r="L257" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="M257" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="N257" s="7"/>
+      <c r="O257" s="16">
+        <f>550*6</f>
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I258" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J258" s="2"/>
+      <c r="K258" s="15">
+        <f>(300*5.5+500*7)-3550</f>
+        <v>1600</v>
+      </c>
+      <c r="M258" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="N258" s="2"/>
+      <c r="O258" s="15">
+        <f>250*6</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I259" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="J259" s="7"/>
+      <c r="K259" s="16">
+        <f>K257-K252</f>
+        <v>150</v>
+      </c>
+      <c r="M259" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="N259" s="7"/>
+      <c r="O259" s="16">
+        <f>O257-K252</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A262" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C262" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J263" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J264" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="K264" s="16"/>
+      <c r="L264" s="16"/>
+      <c r="M264" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N264" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="O264" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J265" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K265" s="8"/>
+      <c r="L265" s="7"/>
+      <c r="M265" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="N265" s="22"/>
+      <c r="O265" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J266" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="K266" s="4"/>
+      <c r="L266" s="7"/>
+      <c r="M266" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="N266" s="22"/>
+      <c r="O266" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J267" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="K267" s="16"/>
+      <c r="L267" s="16"/>
+      <c r="M267" s="8"/>
+      <c r="N267" s="4"/>
+      <c r="O267" s="7"/>
+    </row>
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J268" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K268" s="4"/>
+      <c r="L268" s="7"/>
+      <c r="M268" s="16"/>
+      <c r="N268" s="16"/>
+      <c r="O268" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J269" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K269" s="4"/>
+      <c r="L269" s="7"/>
+      <c r="M269" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="N269" s="16"/>
+      <c r="O269" s="16"/>
+    </row>
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J270" t="s">
+        <v>31</v>
+      </c>
+      <c r="M270" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N270" t="s">
+        <v>154</v>
+      </c>
+      <c r="O270" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J271" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="K271" s="8"/>
+      <c r="L271" s="7"/>
+      <c r="M271" s="16"/>
+      <c r="N271" s="16"/>
+      <c r="O271" s="16"/>
+      <c r="P271" s="27"/>
+    </row>
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A272" s="1"/>
+      <c r="B272" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C272" s="1"/>
+      <c r="D272" s="2"/>
+      <c r="E272" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F272" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G272" s="16"/>
+      <c r="H272" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="J272" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K272" s="4"/>
+      <c r="L272" s="7"/>
+      <c r="O272" s="2"/>
+    </row>
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A273" s="8"/>
+      <c r="B273" s="4"/>
+      <c r="C273" s="4"/>
+      <c r="D273" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="E273" s="16">
+        <v>35</v>
+      </c>
+      <c r="F273" s="8"/>
+      <c r="G273" s="7">
+        <v>35</v>
+      </c>
+      <c r="H273" s="16">
+        <v>35</v>
+      </c>
+      <c r="J273" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="K273" s="8"/>
+      <c r="L273" s="7"/>
+      <c r="M273" s="16"/>
+      <c r="N273" s="16"/>
+      <c r="O273" s="16"/>
+    </row>
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A274" s="8"/>
+      <c r="B274" s="4"/>
+      <c r="C274" s="4"/>
+      <c r="D274" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="E274" s="16">
+        <f>35*M273/100</f>
+        <v>0</v>
+      </c>
+      <c r="F274" s="8"/>
+      <c r="G274" s="7">
+        <f>35*M274/100</f>
+        <v>0</v>
+      </c>
+      <c r="H274" s="16">
+        <f>35*M275/100</f>
+        <v>0</v>
+      </c>
+      <c r="J274" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="K274" s="8"/>
+      <c r="L274" s="7"/>
+      <c r="M274" s="16"/>
+      <c r="N274" s="16"/>
+      <c r="O274" s="16"/>
+    </row>
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A275" s="4"/>
+      <c r="B275" s="4"/>
+      <c r="C275" s="4"/>
+      <c r="D275" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="E275">
+        <v>20</v>
+      </c>
+      <c r="F275" s="8"/>
+      <c r="G275" s="7">
+        <v>20</v>
+      </c>
+      <c r="H275" s="2">
+        <v>20</v>
+      </c>
+      <c r="J275" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="K275" s="8"/>
+      <c r="L275" s="7"/>
+      <c r="M275" s="16"/>
+      <c r="N275" s="16"/>
+      <c r="O275" s="16"/>
+    </row>
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A276" s="8"/>
+      <c r="B276" s="4"/>
+      <c r="C276" s="4"/>
+      <c r="D276" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E276" s="16">
+        <f>20*N273/100</f>
+        <v>0</v>
+      </c>
+      <c r="F276" s="8"/>
+      <c r="G276" s="7">
+        <f>20*N274/100</f>
+        <v>0</v>
+      </c>
+      <c r="H276" s="16">
+        <f>20*N275/100</f>
+        <v>0</v>
+      </c>
+      <c r="J276" s="8"/>
+      <c r="K276" s="4"/>
+      <c r="L276" s="7"/>
+      <c r="M276" s="16"/>
+      <c r="N276" s="16"/>
+      <c r="O276" s="16"/>
+    </row>
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A277" s="8"/>
+      <c r="B277" s="4"/>
+      <c r="C277" s="4"/>
+      <c r="D277" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="E277" s="16">
+        <f>SUM(E273:E276)</f>
+        <v>55</v>
+      </c>
+      <c r="F277" s="8"/>
+      <c r="G277" s="7">
+        <f t="shared" ref="G277" si="2">SUM(G273:G276)</f>
+        <v>55</v>
+      </c>
+      <c r="H277" s="16">
+        <f>SUM(H273:H276)</f>
+        <v>55</v>
+      </c>
+      <c r="J277" s="8"/>
+      <c r="K277" s="4"/>
+      <c r="L277" s="7"/>
+      <c r="M277" s="16"/>
+      <c r="N277" s="16"/>
+      <c r="O277" s="16"/>
+    </row>
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A278" s="8"/>
+      <c r="B278" s="4"/>
+      <c r="C278" s="4"/>
+      <c r="D278" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E278" s="16">
+        <v>0</v>
+      </c>
+      <c r="F278" s="8"/>
+      <c r="G278" s="7">
+        <f>G277*O274/100</f>
+        <v>0</v>
+      </c>
+      <c r="H278" s="7">
+        <f>H277*O275/100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A279" s="1"/>
+      <c r="B279" s="1"/>
+      <c r="C279" s="1"/>
+      <c r="D279" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="E279" s="16">
+        <f>SUM(E277:E278)</f>
+        <v>55</v>
+      </c>
+      <c r="F279" s="8"/>
+      <c r="G279" s="7">
+        <f t="shared" ref="G279:H279" si="3">SUM(G277:G278)</f>
+        <v>55</v>
+      </c>
+      <c r="H279" s="16">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A282" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H284" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="I284" s="16"/>
+      <c r="J284" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="K284" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M284" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="N284" s="7"/>
+      <c r="O284" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="P284" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H285" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="I285" s="16"/>
+      <c r="J285" s="16"/>
+      <c r="K285" s="16"/>
+      <c r="M285" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="N285" s="16"/>
+      <c r="O285" s="16"/>
+      <c r="P285" s="16"/>
+    </row>
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H286" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I286" s="16"/>
+      <c r="J286" s="16"/>
+      <c r="K286" s="16"/>
+      <c r="M286" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="N286" s="16"/>
+      <c r="O286" s="16"/>
+      <c r="P286" s="16"/>
+    </row>
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H287" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I287" s="4"/>
+      <c r="J287" s="7"/>
+      <c r="K287" s="7"/>
+      <c r="M287" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="N287" s="4"/>
+      <c r="O287" s="7"/>
+      <c r="P287" s="7"/>
+    </row>
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H288" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I288" s="16"/>
+      <c r="J288" s="16"/>
+      <c r="K288" s="16"/>
+      <c r="M288" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="N288" s="16"/>
+      <c r="O288" s="16"/>
+      <c r="P288" s="16"/>
+    </row>
+    <row r="289" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J289" s="11"/>
+      <c r="K289" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>